<commit_message>
Binary files `dados.xlsx` and `shape_predictor_68_face_landmarks.dat.bz2` differ.
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,7 +547,22 @@
           <t>juliocamposmachado@gmail.com</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>5511970603441</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Julio</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Julio@Julio.com.br</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>5511970603441</t>
         </is>

</xml_diff>